<commit_message>
Se agrego mas informacion al proceso
</commit_message>
<xml_diff>
--- a/Scraper/recetas.xlsx
+++ b/Scraper/recetas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="95">
   <si>
     <t>Fecha</t>
   </si>
@@ -34,6 +34,18 @@
     <t>url</t>
   </si>
   <si>
+    <t>03/08/2023 17:01</t>
+  </si>
+  <si>
+    <t>03/08/2023 16:01</t>
+  </si>
+  <si>
+    <t>02/08/2023 11:01</t>
+  </si>
+  <si>
+    <t>02/08/2023 07:04</t>
+  </si>
+  <si>
     <t>31/07/2023 09:00</t>
   </si>
   <si>
@@ -82,16 +94,16 @@
     <t>15/07/2023 10:01</t>
   </si>
   <si>
-    <t>13/07/2023 16:00</t>
-  </si>
-  <si>
-    <t>25/07/2023 05:23</t>
-  </si>
-  <si>
-    <t>11/07/2023 15:00</t>
-  </si>
-  <si>
-    <t>11/07/2023 10:18</t>
+    <t>Esta comida callejera italiana, sabrosa y fácil, es mi receta favorita con calabacín</t>
+  </si>
+  <si>
+    <t>Muffins salados de boniato, una receta para chuparse los dedos</t>
+  </si>
+  <si>
+    <t>Refrescante, saciante y sin encender un fuego: esta receta de calabacín es una cena saludable de verano perfecta</t>
+  </si>
+  <si>
+    <t>Así son los nuevos postres veganos de Dia (que no son yogures) con tres bases vegetales diferentes</t>
   </si>
   <si>
     <t>Despedimos el séptimo mes del año en el menú semanal vegetariano del 31 de julio</t>
@@ -142,31 +154,22 @@
     <t>Crujientes de brócoli o smashed broccoli: receta de un picoteo vegetariano, tan saludable como apetecible</t>
   </si>
   <si>
-    <t>Ensalada de pimientos: receta de un clásico del verano, con el truco para que sea aún más delicosa</t>
-  </si>
-  <si>
-    <t>Solo necesitas 10 minutos para preparar esta receta de verano y cenar un plato fresco, saludable y vegetariano</t>
-  </si>
-  <si>
-    <t>Este truco convierte uno de los aperitivos que más nos gustan en una cena completa y saludable</t>
-  </si>
-  <si>
-    <t>Lahanosalata, una clásica ensalada de col griega: receta saludable, fresca e intensa</t>
+    <t>Miguel Ayuso Rejas</t>
   </si>
   <si>
     <t>Inés Vazquez Noya</t>
   </si>
   <si>
+    <t>Liliana Fuchs</t>
+  </si>
+  <si>
     <t>Carmen Tía Alia</t>
   </si>
   <si>
-    <t>Liliana Fuchs</t>
-  </si>
-  <si>
     <t>Pakus</t>
   </si>
   <si>
-    <t>Miguel Ayuso Rejas</t>
+    <t>Harina integral 200 gLevadura química cucharadita1 Sal y pimienta al gusto Boniato cocido161 gLeche o bebida vegetal de almendras, de avena o de soja300 mlAceite de girasol 30 mlEspinaca fresca 50 gGuisantes 30 gComino molido 1 cuchara aproximadamente10 g</t>
   </si>
   <si>
     <t>Queso halloumi 200 gMiel 15 mlSemillas de sésamo 5 g</t>
@@ -202,10 +205,7 @@
     <t>Brócoli cortado en arbolitos1 Queso rallado para espolvorear en cada brócoliPasta de chile picante o copos de chile o guindilla, al gustoAceite de oliva virgen extra para elaborar la salsa picanteSal y pimienta al gusto</t>
   </si>
   <si>
-    <t>Pimiento rojo asado1 Diente de ajo 2 Cebolleta mediaSal gruesa o en escamasAceite de oliva virgen extra</t>
-  </si>
-  <si>
-    <t>Col blanca media cabeza0.5 Cebolla blanca 0.5 Perejil fresco manojo generosoLimón zumo y ralladura1 Sal gruesa pizcaAceite de oliva virgen extra 2 a 3 cucharadasSemillas de sésamo</t>
+    <t>Encender el horno a 190 ºC.En un cuenco mezclar los ingredientes secos: harina integral, levadura química, sal y pimienta. Integrar con un batidor de varilla o un tenedor. Reservar. Por otra parte, en un robot de cocina o licuadora, triturar 100 g de boniato ya cocido con la leche o bebida y aceite de girasol. Pulsar por varios segundos hasta conseguir una bebida liquida de color naranja. Agregar este último al recipiente con la harina e integrar hasta tener una masa homogénea. Momento de agregar la espinaca fresca, los guisantes y los 80 g de boniato restantes en cubitos, más el comino molido. Revolver nuevamente.  Acomodar en molde de muffins de silicona y verter la mezcla anterior sin alcanzar la superficie. De utilizar moldes de acero, pintar con aceite toda la superficie. Cocinar por 30 minutos. Dejar reposar unos 10 minutos antes de desmoldar y disfrutar.</t>
   </si>
   <si>
     <t>Cortamos el queso halloumi en diez piezas de un tamaño aproximado y con forma de lingote. Los ponemos en remojo con abundante agua y los dejamos reposar en la nevera 30-40 minutos. Con esto conseguiremos rebajar un poco el punto de sal que tiene este queso. Secamos los palitos de halloumi con papel absorbente y los ensartamos en brochetas, aunque también los podemos dejar tal cual. Los marcamos en una parrilla bien caliente por todas sus caras. Después los pincelamos con miel y los espolvoreamos con semillas de sésamo. Servimos inmediatamente.</t>
@@ -241,10 +241,16 @@
     <t>Comenzamos cortando el brócoli, para separar los distintos arbolitos. Seguidamente los cocemos con agua y una pizca de sal, dejando que queden bien hechos. Tras cocerlos durante 15 minutos, los escurrimos bien y los repartimos en una bandeja de horno cubierta con papel de hornear. Con un vaso, procedemos a espachurrar o aplastar los arbolitos de brócoli. Mientras, preparamos un aceite picante de chili, diluyendo un poco de pasta de chiles en aceite de oliva. También podemos utilizar copos de chile o utilizar una combinación de aceite con pimentón picante o cualquier especia que nos guste. Untamos a nuestro gusto los arbolitos de brócoli aplastados con ese preparado picante y espolvoreamos con queso parmesano rallado, -sin abusar- procediendo a gratinar en el horno durante 8 minutos a 230ºC. Tras ese tiempo damos la vuelta a los trozos de brócoli y dejamos dentro del horno ya apagado otro par de minutos, para que queden aún más crujientes.   Si los preparamos en airfryer o freidora de aire sin aceite, colocamos los trozos de brócoli ya preparados en la cesta y cocinamos 6-8 minutos a 200ºC revisando a mitad de la cocción para ver cómo va, para evitar que se doren en exceso. En este caso hay que hacerlos en tandas de seis u ocho trozos para que no se toquen unos con otros.</t>
   </si>
   <si>
-    <t>Para hacer esta ensalada partimos de unos buenos pimientos asados, que hemos pelado, despepitado, y separado en tiras. Por cada pimiento añadimos media cebolleta cortada en juliana fina y dos dientes de ajo laminados y cocinados en aceite de oliva virgen extra a baja temperatura, hasta que estén dorados. Dejamos que se enfríen los ajos unos minutos y los echamos sobre la ensalada, junto al aceite aromatizado con ellos. Mezclamos todo y terminamos la ensalada con un poco des sal gruesa o, mejor, unas escamas de sal. Se puede echar también un chorrito de vinagre, pero a mi me gustan sin ningún añadido más.</t>
-  </si>
-  <si>
-    <t>Retirar la primera capa de hojas de la col blanca. Cortar una rodaja en la base para apoyar y facilitar el corte. Cortar cuidadosamente en tiras alargadas y finas. Para ello nos podemos ayudar de una mandolina, o bien hacerlo directamente con un buen cuchillo. Añadir a una ensaladera grande. Agregar una pizca de sal marina gruesa y con las manos hacer un masaje al repollo por unos minutos. Cortar la cebolla en juliana o tiras alargadas y finas, y en crudo agregar al repollo. Añadir la ralladura y zumo de limón, el perejil picado y el aceite de oliva encima de las verduras y revolver bien para integrar. Servir con unas semillas de sésamo por encima.</t>
+    <t>https://www.directoalpaladar.com/recetas-vegetarianas/esta-comida-callejera-italiana-sabrosa-facil-mi-receta-favorita-calabacin</t>
+  </si>
+  <si>
+    <t>https://www.directoalpaladar.com/recetas-vegetarianas/muffins-salados-boniato-receta-para-chuparse-dedos</t>
+  </si>
+  <si>
+    <t>https://www.directoalpaladar.com/recetas-vegetarianas/refrescante-saciante-encender-fuego-esta-receta-calabacin-cena-saludable-verano-perfecta</t>
+  </si>
+  <si>
+    <t>https://www.directoalpaladar.com/recetas-vegetarianas/asi-nuevos-postres-veganos-dia-que-no-yogures-tres-bases-vegetales-diferentes</t>
   </si>
   <si>
     <t>https://www.directoalpaladar.com/recetas-vegetarianas/despedimos-septimo-mes-ano-menu-semanal-vegetariano-31-julio</t>
@@ -293,18 +299,6 @@
   </si>
   <si>
     <t>https://www.directoalpaladar.com/recetas-vegetarianas/receta-crujientes-brocoli-smashed-broccoli-perfectos-para-saludable-picoteo-finde</t>
-  </si>
-  <si>
-    <t>https://www.directoalpaladar.com/recetas-vegetarianas/ensalada-pimientos-receta-clasico-verano-truco-sea-delicosa</t>
-  </si>
-  <si>
-    <t>https://www.directoalpaladar.com/recetario/solo-necesitas-10-minutos-para-preparar-esta-receta-verano-cenar-plato-fresco-saludable-vegetariano</t>
-  </si>
-  <si>
-    <t>https://www.directoalpaladar.com/recetas-vegetarianas/este-truco-convierte-uno-aperitivos-que-nos-gustan-cena-completa-saludable</t>
-  </si>
-  <si>
-    <t>https://www.directoalpaladar.com/recetas-vegetarianas/lahanosalata-clasica-ensalada-col-griega-receta-saludable-fresca-e-intensa</t>
   </si>
 </sst>
 </file>
@@ -712,7 +706,7 @@
         <v>46</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -729,10 +723,10 @@
         <v>51</v>
       </c>
       <c r="E3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -743,16 +737,10 @@
         <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E4" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -763,16 +751,10 @@
         <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -783,10 +765,10 @@
         <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -797,10 +779,16 @@
         <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="D7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" t="s">
+        <v>64</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -814,13 +802,13 @@
         <v>47</v>
       </c>
       <c r="D8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -831,16 +819,16 @@
         <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -851,16 +839,10 @@
         <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -871,16 +853,10 @@
         <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E11" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -891,16 +867,16 @@
         <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E12" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -911,10 +887,16 @@
         <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>47</v>
+      </c>
+      <c r="D13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" t="s">
+        <v>68</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -925,16 +907,16 @@
         <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E14" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -945,16 +927,16 @@
         <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E15" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -965,10 +947,16 @@
         <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="D16" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" t="s">
+        <v>71</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -979,16 +967,10 @@
         <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" t="s">
-        <v>61</v>
-      </c>
-      <c r="E17" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -999,16 +981,16 @@
         <v>42</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E18" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1019,10 +1001,16 @@
         <v>43</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>47</v>
+      </c>
+      <c r="D19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" t="s">
+        <v>73</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1033,10 +1021,10 @@
         <v>44</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1047,16 +1035,16 @@
         <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios en busqueda de la pagina ideal de horoscopos
</commit_message>
<xml_diff>
--- a/Scraper/recetas.xlsx
+++ b/Scraper/recetas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="92">
   <si>
     <t>Fecha</t>
   </si>
@@ -34,6 +34,9 @@
     <t>url</t>
   </si>
   <si>
+    <t>04/08/2023 15:01</t>
+  </si>
+  <si>
     <t>03/08/2023 17:01</t>
   </si>
   <si>
@@ -91,7 +94,7 @@
     <t>17/07/2023 09:23</t>
   </si>
   <si>
-    <t>15/07/2023 10:01</t>
+    <t>Este desayuno con huevos, típico de Oriente Medio, es la cena veraniega perfecta</t>
   </si>
   <si>
     <t>Esta comida callejera italiana, sabrosa y fácil, es mi receta favorita con calabacín</t>
@@ -151,9 +154,6 @@
     <t>Recetas fáciles para atravesar la ola de calor en el menú semanal vegetariano del 17 de julio</t>
   </si>
   <si>
-    <t>Crujientes de brócoli o smashed broccoli: receta de un picoteo vegetariano, tan saludable como apetecible</t>
-  </si>
-  <si>
     <t>Miguel Ayuso Rejas</t>
   </si>
   <si>
@@ -166,9 +166,6 @@
     <t>Carmen Tía Alia</t>
   </si>
   <si>
-    <t>Pakus</t>
-  </si>
-  <si>
     <t>Harina integral 200 gLevadura química cucharadita1 Sal y pimienta al gusto Boniato cocido161 gLeche o bebida vegetal de almendras, de avena o de soja300 mlAceite de girasol 30 mlEspinaca fresca 50 gGuisantes 30 gComino molido 1 cuchara aproximadamente10 g</t>
   </si>
   <si>
@@ -202,9 +199,6 @@
     <t>Hojas verdes 100 gMaíz dulce 50 gManzana roja o verde1 Miel 1 cucharadaVinagre de vino blanco 1 cucharadaAceite de oliva virgen extra 2 a 3 cucharadasSal y pimienta al gusto Orégano seco opcionalSemillas de calabaza opcional - para la decoración</t>
   </si>
   <si>
-    <t>Brócoli cortado en arbolitos1 Queso rallado para espolvorear en cada brócoliPasta de chile picante o copos de chile o guindilla, al gustoAceite de oliva virgen extra para elaborar la salsa picanteSal y pimienta al gusto</t>
-  </si>
-  <si>
     <t>Encender el horno a 190 ºC.En un cuenco mezclar los ingredientes secos: harina integral, levadura química, sal y pimienta. Integrar con un batidor de varilla o un tenedor. Reservar. Por otra parte, en un robot de cocina o licuadora, triturar 100 g de boniato ya cocido con la leche o bebida y aceite de girasol. Pulsar por varios segundos hasta conseguir una bebida liquida de color naranja. Agregar este último al recipiente con la harina e integrar hasta tener una masa homogénea. Momento de agregar la espinaca fresca, los guisantes y los 80 g de boniato restantes en cubitos, más el comino molido. Revolver nuevamente.  Acomodar en molde de muffins de silicona y verter la mezcla anterior sin alcanzar la superficie. De utilizar moldes de acero, pintar con aceite toda la superficie. Cocinar por 30 minutos. Dejar reposar unos 10 minutos antes de desmoldar y disfrutar.</t>
   </si>
   <si>
@@ -238,7 +232,7 @@
     <t>Lavar las hojas verdes y colocar en una ensaladera. Agregar los granos de maíz dulce. Lavar la manzana y cortar en dados o finas láminas. Añadir a la ensaladera. Preparar el aliño en un cuenco separado con sal, pimienta, orégano seco, vinagre de vino, miel y aceite de oliva. Revolver hasta emulsionar. Volcar sobre las verduras frescas, y revolver para integrar. Servir y terminar con unas pipas de calabaza en la superficie.</t>
   </si>
   <si>
-    <t>Comenzamos cortando el brócoli, para separar los distintos arbolitos. Seguidamente los cocemos con agua y una pizca de sal, dejando que queden bien hechos. Tras cocerlos durante 15 minutos, los escurrimos bien y los repartimos en una bandeja de horno cubierta con papel de hornear. Con un vaso, procedemos a espachurrar o aplastar los arbolitos de brócoli. Mientras, preparamos un aceite picante de chili, diluyendo un poco de pasta de chiles en aceite de oliva. También podemos utilizar copos de chile o utilizar una combinación de aceite con pimentón picante o cualquier especia que nos guste. Untamos a nuestro gusto los arbolitos de brócoli aplastados con ese preparado picante y espolvoreamos con queso parmesano rallado, -sin abusar- procediendo a gratinar en el horno durante 8 minutos a 230ºC. Tras ese tiempo damos la vuelta a los trozos de brócoli y dejamos dentro del horno ya apagado otro par de minutos, para que queden aún más crujientes.   Si los preparamos en airfryer o freidora de aire sin aceite, colocamos los trozos de brócoli ya preparados en la cesta y cocinamos 6-8 minutos a 200ºC revisando a mitad de la cocción para ver cómo va, para evitar que se doren en exceso. En este caso hay que hacerlos en tandas de seis u ocho trozos para que no se toquen unos con otros.</t>
+    <t>https://www.directoalpaladar.com/recetas-vegetarianas/este-desayuno-huevos-tipico-oriente-medio-cena-veraniega-perfecta</t>
   </si>
   <si>
     <t>https://www.directoalpaladar.com/recetas-vegetarianas/esta-comida-callejera-italiana-sabrosa-facil-mi-receta-favorita-calabacin</t>
@@ -296,9 +290,6 @@
   </si>
   <si>
     <t>https://www.directoalpaladar.com/recetas-vegetarianas/recetas-faciles-para-atravezar-ola-calor-menu-semanal-vegetariano-17-julio</t>
-  </si>
-  <si>
-    <t>https://www.directoalpaladar.com/recetas-vegetarianas/receta-crujientes-brocoli-smashed-broccoli-perfectos-para-saludable-picoteo-finde</t>
   </si>
 </sst>
 </file>
@@ -706,7 +697,7 @@
         <v>46</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -717,16 +708,10 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -737,10 +722,16 @@
         <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>47</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" t="s">
+        <v>61</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -754,7 +745,7 @@
         <v>48</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -765,10 +756,10 @@
         <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -779,16 +770,10 @@
         <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" t="s">
-        <v>52</v>
-      </c>
-      <c r="E7" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -799,16 +784,16 @@
         <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -819,16 +804,16 @@
         <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -839,10 +824,16 @@
         <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>49</v>
+      </c>
+      <c r="D10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" t="s">
+        <v>64</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -853,10 +844,10 @@
         <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -867,16 +858,10 @@
         <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" t="s">
-        <v>55</v>
-      </c>
-      <c r="E12" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -887,16 +872,16 @@
         <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -910,13 +895,13 @@
         <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E14" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -930,13 +915,13 @@
         <v>47</v>
       </c>
       <c r="D15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E15" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -950,13 +935,13 @@
         <v>47</v>
       </c>
       <c r="D16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E16" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -967,10 +952,16 @@
         <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>47</v>
+      </c>
+      <c r="D17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" t="s">
+        <v>69</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -981,16 +972,10 @@
         <v>42</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" t="s">
-        <v>60</v>
-      </c>
-      <c r="E18" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1004,13 +989,13 @@
         <v>47</v>
       </c>
       <c r="D19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1023,8 +1008,14 @@
       <c r="C20" t="s">
         <v>47</v>
       </c>
+      <c r="D20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" t="s">
+        <v>71</v>
+      </c>
       <c r="F20" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1035,16 +1026,10 @@
         <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" t="s">
-        <v>62</v>
-      </c>
-      <c r="E21" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se agrego el scraper de horoscopos, aun se debe trabajar en corregir el formato de la informacion
</commit_message>
<xml_diff>
--- a/Scraper/recetas.xlsx
+++ b/Scraper/recetas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="94">
   <si>
     <t>Fecha</t>
   </si>
@@ -34,6 +34,9 @@
     <t>url</t>
   </si>
   <si>
+    <t>06/08/2023 17:00</t>
+  </si>
+  <si>
     <t>04/08/2023 15:01</t>
   </si>
   <si>
@@ -91,7 +94,7 @@
     <t>17/07/2023 10:01</t>
   </si>
   <si>
-    <t>17/07/2023 09:23</t>
+    <t>Paté rosa de remolacha y tofu, una receta para decorar la mesa</t>
   </si>
   <si>
     <t>Este desayuno con huevos, típico de Oriente Medio, es la cena veraniega perfecta</t>
@@ -151,21 +154,21 @@
     <t>Ensalada de lechuga, maíz dulce y manzana, una receta de verano de Karlos Arguiñano</t>
   </si>
   <si>
-    <t>Recetas fáciles para atravesar la ola de calor en el menú semanal vegetariano del 17 de julio</t>
+    <t>Inés Vazquez Noya</t>
   </si>
   <si>
     <t>Miguel Ayuso Rejas</t>
   </si>
   <si>
-    <t>Inés Vazquez Noya</t>
-  </si>
-  <si>
     <t>Liliana Fuchs</t>
   </si>
   <si>
     <t>Carmen Tía Alia</t>
   </si>
   <si>
+    <t>Tofu blando 100 gRemolacha cocida 50 gAgua de la remolacha - 2 cucharadasComino molido 10 gSal y pimienta al gusto</t>
+  </si>
+  <si>
     <t>Harina integral 200 gLevadura química cucharadita1 Sal y pimienta al gusto Boniato cocido161 gLeche o bebida vegetal de almendras, de avena o de soja300 mlAceite de girasol 30 mlEspinaca fresca 50 gGuisantes 30 gComino molido 1 cuchara aproximadamente10 g</t>
   </si>
   <si>
@@ -199,6 +202,9 @@
     <t>Hojas verdes 100 gMaíz dulce 50 gManzana roja o verde1 Miel 1 cucharadaVinagre de vino blanco 1 cucharadaAceite de oliva virgen extra 2 a 3 cucharadasSal y pimienta al gusto Orégano seco opcionalSemillas de calabaza opcional - para la decoración</t>
   </si>
   <si>
+    <t>Primero, tomar el tofu y quitar el líquido del envase. Presionar encima con un plato, de tal forma que vaya soltando todo el líquido y luego escurrir entre dos hojas de papel de cocina. Cortar en cubos o romper con las manos. En un robot de cocina, agregar las porciones de tofu, junto a la remolacha troceada, el comino molido, la sal, la pimienta y la cucharada de agua de la remolacha. Triturar hasta obtener una pasta homogénea.  De ser necesario, agregar 1 a 2 cucharaditas más de agua, si ves que la preparación necesita mas hidratación hasta alcanzar una textura cremosa.</t>
+  </si>
+  <si>
     <t>Encender el horno a 190 ºC.En un cuenco mezclar los ingredientes secos: harina integral, levadura química, sal y pimienta. Integrar con un batidor de varilla o un tenedor. Reservar. Por otra parte, en un robot de cocina o licuadora, triturar 100 g de boniato ya cocido con la leche o bebida y aceite de girasol. Pulsar por varios segundos hasta conseguir una bebida liquida de color naranja. Agregar este último al recipiente con la harina e integrar hasta tener una masa homogénea. Momento de agregar la espinaca fresca, los guisantes y los 80 g de boniato restantes en cubitos, más el comino molido. Revolver nuevamente.  Acomodar en molde de muffins de silicona y verter la mezcla anterior sin alcanzar la superficie. De utilizar moldes de acero, pintar con aceite toda la superficie. Cocinar por 30 minutos. Dejar reposar unos 10 minutos antes de desmoldar y disfrutar.</t>
   </si>
   <si>
@@ -232,6 +238,9 @@
     <t>Lavar las hojas verdes y colocar en una ensaladera. Agregar los granos de maíz dulce. Lavar la manzana y cortar en dados o finas láminas. Añadir a la ensaladera. Preparar el aliño en un cuenco separado con sal, pimienta, orégano seco, vinagre de vino, miel y aceite de oliva. Revolver hasta emulsionar. Volcar sobre las verduras frescas, y revolver para integrar. Servir y terminar con unas pipas de calabaza en la superficie.</t>
   </si>
   <si>
+    <t>https://www.directoalpaladar.com/recetas-vegetarianas/pate-rosa-remolacha-tofu-receta-para-decorar-mesa</t>
+  </si>
+  <si>
     <t>https://www.directoalpaladar.com/recetas-vegetarianas/este-desayuno-huevos-tipico-oriente-medio-cena-veraniega-perfecta</t>
   </si>
   <si>
@@ -287,9 +296,6 @@
   </si>
   <si>
     <t>https://www.directoalpaladar.com/recetas-vegetarianas/ensalada-lechuga-maiz-dulce-manzana-receta-verano-arguinano</t>
-  </si>
-  <si>
-    <t>https://www.directoalpaladar.com/recetas-vegetarianas/recetas-faciles-para-atravezar-ola-calor-menu-semanal-vegetariano-17-julio</t>
   </si>
 </sst>
 </file>
@@ -696,8 +702,14 @@
       <c r="C2" t="s">
         <v>46</v>
       </c>
+      <c r="D2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" t="s">
+        <v>62</v>
+      </c>
       <c r="F2" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -708,10 +720,10 @@
         <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -724,14 +736,8 @@
       <c r="C4" t="s">
         <v>47</v>
       </c>
-      <c r="D4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" t="s">
-        <v>61</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -742,10 +748,16 @@
         <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>46</v>
+      </c>
+      <c r="D5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" t="s">
+        <v>63</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -759,7 +771,7 @@
         <v>48</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -770,10 +782,10 @@
         <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -784,16 +796,10 @@
         <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E8" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -804,16 +810,16 @@
         <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D9" t="s">
         <v>52</v>
       </c>
       <c r="E9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -824,16 +830,16 @@
         <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D10" t="s">
         <v>53</v>
       </c>
       <c r="E10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -844,10 +850,16 @@
         <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>47</v>
+        <v>49</v>
+      </c>
+      <c r="D11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" t="s">
+        <v>66</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -858,10 +870,10 @@
         <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -872,16 +884,10 @@
         <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -892,16 +898,16 @@
         <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D14" t="s">
         <v>55</v>
       </c>
       <c r="E14" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -912,16 +918,16 @@
         <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D15" t="s">
         <v>56</v>
       </c>
       <c r="E15" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -932,16 +938,16 @@
         <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D16" t="s">
         <v>57</v>
       </c>
       <c r="E16" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -952,16 +958,16 @@
         <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D17" t="s">
         <v>58</v>
       </c>
       <c r="E17" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -972,10 +978,16 @@
         <v>42</v>
       </c>
       <c r="C18" t="s">
-        <v>48</v>
+        <v>46</v>
+      </c>
+      <c r="D18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" t="s">
+        <v>71</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -986,16 +998,10 @@
         <v>43</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" t="s">
-        <v>59</v>
-      </c>
-      <c r="E19" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1006,16 +1012,16 @@
         <v>44</v>
       </c>
       <c r="C20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D20" t="s">
         <v>60</v>
       </c>
       <c r="E20" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1026,10 +1032,16 @@
         <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>46</v>
+      </c>
+      <c r="D21" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" t="s">
+        <v>73</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>